<commit_message>
Almost Done with screenshot not showing in report problem
</commit_message>
<xml_diff>
--- a/test_cases/salesforce_test_cases.xlsx
+++ b/test_cases/salesforce_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BhartiPr\PycharmProjects\SalesforceDemo\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306D1262-C0AD-42C6-9FA0-E729A1AEF804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F25DB8-DD68-4CA2-AB90-C4929F7FDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Test ID</t>
   </si>
@@ -150,10 +150,37 @@
     <t>store value from Opportunity Name as opportunity_name</t>
   </si>
   <si>
-    <t>verify xpath=//lightning-formatted-text[text()='${opportunity_name}'] is available</t>
-  </si>
-  <si>
-    <t>Step15</t>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Delete a Opportunity</t>
+  </si>
+  <si>
+    <t>Delete a Opportunity which previously made</t>
+  </si>
+  <si>
+    <t>click Opportunity record with value="Try1"</t>
+  </si>
+  <si>
+    <t>click Opprotunity show Options</t>
+  </si>
+  <si>
+    <t>click Opportunity Delete</t>
+  </si>
+  <si>
+    <t>click Opportunity Delete Confirm</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Edit a Opportunity</t>
+  </si>
+  <si>
+    <t>click Opportunity Edit</t>
+  </si>
+  <si>
+    <t>fill Opportunity Name with Tryedit</t>
   </si>
 </sst>
 </file>
@@ -480,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,7 +523,7 @@
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,11 +578,8 @@
       <c r="R1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -584,7 +608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="116" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -639,8 +663,90 @@
       <c r="R3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="S3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>